<commit_message>
Full Data Set Now in Use. Cleaned Up Alot of the the Program.
</commit_message>
<xml_diff>
--- a/input_data_2.xlsx
+++ b/input_data_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\Healthy\Healthy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7C729C5-EBCB-4604-ACC3-3CDC6029B219}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{67758334-890B-4A57-8B9A-47090F396911}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="47" uniqueCount="47">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="80" uniqueCount="80">
   <si>
     <t>site</t>
   </si>
@@ -168,13 +168,112 @@
   </si>
   <si>
     <t>Lung Pleuracy</t>
+  </si>
+  <si>
+    <t>Vaccination flu</t>
+  </si>
+  <si>
+    <t>Vaccination paeds</t>
+  </si>
+  <si>
+    <t>Vaccination travel</t>
+  </si>
+  <si>
+    <t>Mental Health depression</t>
+  </si>
+  <si>
+    <t>Mental Health bipolar</t>
+  </si>
+  <si>
+    <t>Mental Health anxiety</t>
+  </si>
+  <si>
+    <t>Mental Health stress</t>
+  </si>
+  <si>
+    <t>Brain Dementia</t>
+  </si>
+  <si>
+    <t>Brain Stroke</t>
+  </si>
+  <si>
+    <t>Falls minor</t>
+  </si>
+  <si>
+    <t>Falls medium</t>
+  </si>
+  <si>
+    <t>Falls major</t>
+  </si>
+  <si>
+    <t>Muscular minor</t>
+  </si>
+  <si>
+    <t>Muscular medium</t>
+  </si>
+  <si>
+    <t>Muscular major</t>
+  </si>
+  <si>
+    <t>Other trauma minor</t>
+  </si>
+  <si>
+    <t>Other trauma medium</t>
+  </si>
+  <si>
+    <t>Other trauma major</t>
+  </si>
+  <si>
+    <t>Arthritis Osteo</t>
+  </si>
+  <si>
+    <t>Arthritis Rheumatoid</t>
+  </si>
+  <si>
+    <t>Rehabilitation</t>
+  </si>
+  <si>
+    <t>Cancer Brain</t>
+  </si>
+  <si>
+    <t>Cancer Breast</t>
+  </si>
+  <si>
+    <t>Cancer ENT</t>
+  </si>
+  <si>
+    <t>Cancer UGI</t>
+  </si>
+  <si>
+    <t>Cancer LGI</t>
+  </si>
+  <si>
+    <t>Cancer Liver</t>
+  </si>
+  <si>
+    <t>Cancer Kidney</t>
+  </si>
+  <si>
+    <t>Cancer Pancreas</t>
+  </si>
+  <si>
+    <t>Cancer Blood</t>
+  </si>
+  <si>
+    <t>Bowel Disorders</t>
+  </si>
+  <si>
+    <t>Gynaecology</t>
+  </si>
+  <si>
+    <t>Paeds General</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -187,13 +286,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,10 +319,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -525,10 +637,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -662,7 +774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -832,14 +944,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -881,306 +995,1560 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>189</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1701</v>
       </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>729</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>2187</v>
       </c>
-      <c r="D3" s="2">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2">
-        <v>6</v>
-      </c>
-      <c r="H3" s="2">
-        <v>4</v>
-      </c>
-      <c r="I3" s="2">
-        <v>3</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1897</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>1897</v>
       </c>
-      <c r="D4" s="2">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>1407</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>8442</v>
       </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>6</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="D5" s="3">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2</v>
+      </c>
+      <c r="L5" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>737</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>737</v>
       </c>
-      <c r="D6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2">
-        <v>6</v>
-      </c>
-      <c r="H6" s="2">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2</v>
+      </c>
+      <c r="L6" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>1200</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>9600</v>
       </c>
-      <c r="D7" s="2">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2">
-        <v>6</v>
-      </c>
-      <c r="H7" s="2">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
+      <c r="L7" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>1867</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>14936</v>
       </c>
-      <c r="D8" s="2">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2">
-        <v>6</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2">
-        <v>3</v>
-      </c>
-      <c r="J8" s="2">
-        <v>2</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2</v>
+      </c>
+      <c r="L8" s="3">
         <v>1.01</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>1691</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>8455</v>
       </c>
-      <c r="D9" s="2">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2">
-        <v>8</v>
-      </c>
-      <c r="G9" s="2">
-        <v>6</v>
-      </c>
-      <c r="H9" s="2">
-        <v>4</v>
-      </c>
-      <c r="I9" s="2">
-        <v>3</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3">
+        <v>981</v>
+      </c>
+      <c r="C10" s="3">
+        <v>981</v>
+      </c>
+      <c r="D10" s="3">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="3">
+        <v>748</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6732</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="3">
+        <v>782</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2346</v>
+      </c>
+      <c r="D12" s="3">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>6</v>
+      </c>
+      <c r="H12" s="3">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3">
+        <v>993</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4965</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1695</v>
+      </c>
+      <c r="C14" s="3">
+        <v>13560</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>6</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="3">
+        <v>318</v>
+      </c>
+      <c r="C15" s="3">
+        <v>318</v>
+      </c>
+      <c r="D15" s="3">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1465</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5860</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3">
+        <v>934</v>
+      </c>
+      <c r="C17" s="3">
+        <v>6538</v>
+      </c>
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="3">
+        <v>652</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3">
+        <v>6</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3">
+        <v>470</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3760</v>
+      </c>
+      <c r="D19" s="3">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3">
+        <v>890</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5340</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <v>6</v>
+      </c>
+      <c r="H20" s="3">
+        <v>4</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1482</v>
+      </c>
+      <c r="C21" s="3">
+        <v>7410</v>
+      </c>
+      <c r="D21" s="3">
+        <v>10</v>
+      </c>
+      <c r="E21" s="3">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1882</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8</v>
+      </c>
+      <c r="G22" s="3">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="3">
+        <v>395</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2370</v>
+      </c>
+      <c r="D23" s="3">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7</v>
+      </c>
+      <c r="F23" s="3">
+        <v>8</v>
+      </c>
+      <c r="G23" s="3">
+        <v>6</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1868</v>
+      </c>
+      <c r="C24" s="3">
+        <v>9340</v>
+      </c>
+      <c r="D24" s="3">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>6</v>
+      </c>
+      <c r="H24" s="3">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="3">
+        <v>650</v>
+      </c>
+      <c r="C25" s="3">
+        <v>650</v>
+      </c>
+      <c r="D25" s="3">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3">
+        <v>7</v>
+      </c>
+      <c r="F25" s="3">
+        <v>8</v>
+      </c>
+      <c r="G25" s="3">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3">
+        <v>4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>3</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>2</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3">
+        <v>730</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2920</v>
+      </c>
+      <c r="D26" s="3">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2</v>
+      </c>
+      <c r="K26" s="3">
+        <v>2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="3">
+        <v>980</v>
+      </c>
+      <c r="C27" s="3">
+        <v>6860</v>
+      </c>
+      <c r="D27" s="3">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>3</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3">
+        <v>2</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="3">
+        <v>899</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1798</v>
+      </c>
+      <c r="D28" s="3">
+        <v>10</v>
+      </c>
+      <c r="E28" s="3">
+        <v>7</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8</v>
+      </c>
+      <c r="G28" s="3">
+        <v>6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>4</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3">
+        <v>2</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1014</v>
+      </c>
+      <c r="C29" s="3">
+        <v>8112</v>
+      </c>
+      <c r="D29" s="3">
+        <v>10</v>
+      </c>
+      <c r="E29" s="3">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3">
+        <v>8</v>
+      </c>
+      <c r="G29" s="3">
+        <v>6</v>
+      </c>
+      <c r="H29" s="3">
+        <v>4</v>
+      </c>
+      <c r="I29" s="3">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2</v>
+      </c>
+      <c r="K29" s="3">
+        <v>2</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1207</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1207</v>
+      </c>
+      <c r="D30" s="3">
+        <v>10</v>
+      </c>
+      <c r="E30" s="3">
+        <v>7</v>
+      </c>
+      <c r="F30" s="3">
+        <v>8</v>
+      </c>
+      <c r="G30" s="3">
+        <v>6</v>
+      </c>
+      <c r="H30" s="3">
+        <v>4</v>
+      </c>
+      <c r="I30" s="3">
+        <v>3</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1867</v>
+      </c>
+      <c r="C31" s="3">
+        <v>18670</v>
+      </c>
+      <c r="D31" s="3">
+        <v>10</v>
+      </c>
+      <c r="E31" s="3">
+        <v>7</v>
+      </c>
+      <c r="F31" s="3">
+        <v>8</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>4</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2</v>
+      </c>
+      <c r="L31" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1914</v>
+      </c>
+      <c r="C32" s="3">
+        <v>17226</v>
+      </c>
+      <c r="D32" s="3">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3">
+        <v>8</v>
+      </c>
+      <c r="G32" s="3">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3">
+        <v>4</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="3">
+        <v>557</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4456</v>
+      </c>
+      <c r="D33" s="3">
+        <v>10</v>
+      </c>
+      <c r="E33" s="3">
+        <v>7</v>
+      </c>
+      <c r="F33" s="3">
+        <v>8</v>
+      </c>
+      <c r="G33" s="3">
+        <v>6</v>
+      </c>
+      <c r="H33" s="3">
+        <v>4</v>
+      </c>
+      <c r="I33" s="3">
+        <v>3</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2</v>
+      </c>
+      <c r="K33" s="3">
+        <v>2</v>
+      </c>
+      <c r="L33" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1887</v>
+      </c>
+      <c r="C34" s="3">
+        <v>15096</v>
+      </c>
+      <c r="D34" s="3">
+        <v>10</v>
+      </c>
+      <c r="E34" s="3">
+        <v>7</v>
+      </c>
+      <c r="F34" s="3">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>4</v>
+      </c>
+      <c r="I34" s="3">
+        <v>3</v>
+      </c>
+      <c r="J34" s="3">
+        <v>2</v>
+      </c>
+      <c r="K34" s="3">
+        <v>2</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1307</v>
+      </c>
+      <c r="C35" s="3">
+        <v>7842</v>
+      </c>
+      <c r="D35" s="3">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
+        <v>7</v>
+      </c>
+      <c r="F35" s="3">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3">
+        <v>6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>4</v>
+      </c>
+      <c r="I35" s="3">
+        <v>3</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2</v>
+      </c>
+      <c r="K35" s="3">
+        <v>2</v>
+      </c>
+      <c r="L35" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="3">
+        <v>604</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1812</v>
+      </c>
+      <c r="D36" s="3">
+        <v>10</v>
+      </c>
+      <c r="E36" s="3">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>4</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>2</v>
+      </c>
+      <c r="K36" s="3">
+        <v>2</v>
+      </c>
+      <c r="L36" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1460</v>
+      </c>
+      <c r="C37" s="3">
+        <v>14600</v>
+      </c>
+      <c r="D37" s="3">
+        <v>10</v>
+      </c>
+      <c r="E37" s="3">
+        <v>7</v>
+      </c>
+      <c r="F37" s="3">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4</v>
+      </c>
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2</v>
+      </c>
+      <c r="L37" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="3">
+        <v>679</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3">
+        <v>7</v>
+      </c>
+      <c r="F38" s="3">
+        <v>8</v>
+      </c>
+      <c r="G38" s="3">
+        <v>6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>4</v>
+      </c>
+      <c r="I38" s="3">
+        <v>3</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2</v>
+      </c>
+      <c r="K38" s="3">
+        <v>2</v>
+      </c>
+      <c r="L38" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3">
+        <v>338</v>
+      </c>
+      <c r="C39" s="3">
+        <v>3380</v>
+      </c>
+      <c r="D39" s="3">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3">
+        <v>7</v>
+      </c>
+      <c r="F39" s="3">
+        <v>8</v>
+      </c>
+      <c r="G39" s="3">
+        <v>6</v>
+      </c>
+      <c r="H39" s="3">
+        <v>4</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3</v>
+      </c>
+      <c r="J39" s="3">
+        <v>2</v>
+      </c>
+      <c r="K39" s="3">
+        <v>2</v>
+      </c>
+      <c r="L39" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1597</v>
+      </c>
+      <c r="C40" s="3">
+        <v>12776</v>
+      </c>
+      <c r="D40" s="3">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3">
+        <v>7</v>
+      </c>
+      <c r="F40" s="3">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3">
+        <v>6</v>
+      </c>
+      <c r="H40" s="3">
+        <v>4</v>
+      </c>
+      <c r="I40" s="3">
+        <v>3</v>
+      </c>
+      <c r="J40" s="3">
+        <v>2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>2</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1726</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3">
+        <v>7</v>
+      </c>
+      <c r="F41" s="3">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3">
+        <v>4</v>
+      </c>
+      <c r="I41" s="3">
+        <v>3</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2</v>
+      </c>
+      <c r="K41" s="3">
+        <v>2</v>
+      </c>
+      <c r="L41" s="3">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="3">
+        <v>820</v>
+      </c>
+      <c r="C42" s="3">
+        <v>4100</v>
+      </c>
+      <c r="D42" s="3">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3">
+        <v>7</v>
+      </c>
+      <c r="F42" s="3">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3">
+        <v>6</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4</v>
+      </c>
+      <c r="I42" s="3">
+        <v>3</v>
+      </c>
+      <c r="J42" s="3">
+        <v>2</v>
+      </c>
+      <c r="K42" s="3">
+        <v>2</v>
+      </c>
+      <c r="L42" s="3">
         <v>1.01</v>
       </c>
     </row>

</xml_diff>